<commit_message>
Capstone Progress Update. Pick up at data intro and conclusions. Also need a more in-depth classifier discussion.
</commit_message>
<xml_diff>
--- a/Unit6_Capstone_Project/classifier_timing_analysis.xlsx
+++ b/Unit6_Capstone_Project/classifier_timing_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeffrey\Documents\GitHub\MachineLearning\Unit6_Capstone_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE7B270-57F1-48F5-BAE1-5D545954FE99}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF17B476-EDC2-49BD-AC01-55CE367B80DF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="42840" windowHeight="11280" xr2:uid="{DE6938C6-DC07-4314-9C4E-FCE5B8C8DF83}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="42840" windowHeight="11280" activeTab="3" xr2:uid="{DE6938C6-DC07-4314-9C4E-FCE5B8C8DF83}"/>
   </bookViews>
   <sheets>
     <sheet name="multiple_linear_regression_time" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="18">
   <si>
     <t>Time</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>Score:</t>
+  </si>
+  <si>
+    <t>accuracy</t>
+  </si>
+  <si>
+    <t>Support</t>
+  </si>
+  <si>
+    <t>Vector</t>
+  </si>
+  <si>
+    <t>Machine</t>
   </si>
 </sst>
 </file>
@@ -423,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A490FAD-93E6-40BB-ADF6-BABDA8E072EE}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,7 +476,7 @@
   <dimension ref="A1:L99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1599,7 +1611,7 @@
   <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K30" sqref="K30:N30"/>
+      <selection activeCell="L53" sqref="L53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1969,7 +1981,7 @@
         <v>0.378613471984863</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -1980,7 +1992,7 @@
         <v>0.36562466621398898</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -1991,7 +2003,7 @@
         <v>0.371619462966918</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -2002,7 +2014,7 @@
         <v>0.37461662292480402</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>0</v>
       </c>
@@ -2012,8 +2024,26 @@
       <c r="C36">
         <v>0.37161970138549799</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="I36" t="s">
+        <v>7</v>
+      </c>
+      <c r="J36" t="s">
+        <v>8</v>
+      </c>
+      <c r="K36" t="s">
+        <v>9</v>
+      </c>
+      <c r="L36" t="s">
+        <v>14</v>
+      </c>
+      <c r="M36" t="s">
+        <v>10</v>
+      </c>
+      <c r="N36">
+        <v>0.61723163841799999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -2024,7 +2054,7 @@
         <v>0.37861299514770502</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>0</v>
       </c>
@@ -2035,7 +2065,7 @@
         <v>0.37961125373840299</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>0</v>
       </c>
@@ -2046,7 +2076,7 @@
         <v>0.37961173057556102</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>0</v>
       </c>
@@ -2057,7 +2087,7 @@
         <v>0.38260817527770902</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -2068,7 +2098,7 @@
         <v>0.37961125373840299</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>0</v>
       </c>
@@ -2079,7 +2109,7 @@
         <v>0.38660430908203097</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>0</v>
       </c>
@@ -2090,7 +2120,7 @@
         <v>0.389601230621337</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>0</v>
       </c>
@@ -2101,7 +2131,7 @@
         <v>0.38760256767272899</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -2112,7 +2142,7 @@
         <v>0.38860177993774397</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>0</v>
       </c>
@@ -2123,7 +2153,7 @@
         <v>0.39159893989562899</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>0</v>
       </c>
@@ -2134,7 +2164,7 @@
         <v>0.39159893989562899</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>0</v>
       </c>
@@ -2163,15 +2193,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A80B37A1-D54B-4752-8EBC-D05DC28F2558}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2179,10 +2209,10 @@
         <v>1</v>
       </c>
       <c r="C1">
-        <v>11.541184425354</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>11.7909286022186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2190,10 +2220,10 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>11.4462809562683</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>11.873843908309899</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2201,20 +2231,20 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>11.5102152824401</v>
+        <v>11.7439749240875</v>
       </c>
       <c r="H3" t="s">
         <v>4</v>
       </c>
       <c r="I3">
         <f>SUM(C:C)/COUNT(C:C)</f>
-        <v>11.484741497039749</v>
+        <v>11.83311466609725</v>
       </c>
       <c r="J3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2222,10 +2252,10 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>11.4852414131164</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>11.5901336669921</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -2233,10 +2263,28 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>11.451276063919</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>12.1445662975311</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5">
+        <v>0.62358757062100001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -2244,10 +2292,10 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>11.5032227039337</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>11.674047708511299</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -2255,10 +2303,10 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>11.4422841072082</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>11.915800333023</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -2266,10 +2314,10 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>11.4892365932464</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>11.998715400695801</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -2277,10 +2325,10 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>11.4892370700836</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>12.008705139160099</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -2288,7 +2336,458 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>11.489236354827799</v>
+        <v>11.798919916152901</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>12.0826294422149</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>11.876840353012</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>11.8888278007507</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>11.9907236099243</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>11.8888278007507</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>11.811906337738</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>12.009704113006499</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>12.323382616043</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>12.0067074298858</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>12.0536587238311</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>12.058655261993399</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>11.8758416175842</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>11.8428742885589</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>11.947767257690399</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>11.9747400283813</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>11.659062147140499</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>11.7389824390411</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>11.6400814056396</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>11.9567582607269</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>11.5671570301055</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>11.5671570301055</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>11.7859332561492</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>11.557167768478299</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>11.7389817237854</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <v>11.7709486484527</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>11.714007139205901</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <v>11.703019142150801</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>11.9108042716979</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>11.790927648544301</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>11.761957645416199</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>11.7829363346099</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>11.6490733623504</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>11.7759437561035</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>11.77894282341</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>11.7140069007873</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>11.7030179500579</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>11.655067205429001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48">
+        <v>11.6850366592407</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>11.680042028427099</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>11.632089853286701</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>12.3970229625701</v>
       </c>
     </row>
   </sheetData>

</xml_diff>